<commit_message>
Rearranged data management subsections for clarity, file size data in excel sheet (to be inserted into document)
</commit_message>
<xml_diff>
--- a/thesis/data and charts.xlsx
+++ b/thesis/data and charts.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10480" yWindow="340" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25580" windowHeight="28280" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="inserts" sheetId="1" r:id="rId1"/>
+    <sheet name="sizes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,12 +20,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Number of sequences (paired end)</t>
   </si>
   <si>
     <t>Time to insert (seconds)</t>
+  </si>
+  <si>
+    <t>Original file size</t>
+  </si>
+  <si>
+    <t>Size of database after insert</t>
+  </si>
+  <si>
+    <t>Number of sequences</t>
+  </si>
+  <si>
+    <t>34.24 GB</t>
+  </si>
+  <si>
+    <t>68.12 GB</t>
+  </si>
+  <si>
+    <t>743 MB</t>
+  </si>
+  <si>
+    <t>1486 MB</t>
+  </si>
+  <si>
+    <t>2.98 GB</t>
+  </si>
+  <si>
+    <t>5.94 GB</t>
+  </si>
+  <si>
+    <t>11.88 GB</t>
+  </si>
+  <si>
+    <t>23.78 GB</t>
+  </si>
+  <si>
+    <t>47.56 GB</t>
+  </si>
+  <si>
+    <t>371.4 MB</t>
+  </si>
+  <si>
+    <t>258.6 MB</t>
+  </si>
+  <si>
+    <t>517.2 MB</t>
+  </si>
+  <si>
+    <t>1054.72 MB</t>
   </si>
 </sst>
 </file>
@@ -103,7 +152,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>inserts!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -115,7 +164,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:f>inserts!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -148,7 +197,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$9</c:f>
+              <c:f>inserts!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -270,6 +319,11 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -283,15 +337,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
+      <xdr:colOff>596900</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -637,7 +691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
@@ -724,4 +778,124 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>500000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>1000000</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>2000000</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4000000</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>8000000</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>16000000</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>32000000</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>64000000</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>91000000</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added file size table and chart (incomplete)
</commit_message>
<xml_diff>
--- a/thesis/data and charts.xlsx
+++ b/thesis/data and charts.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Number of sequences (paired end)</t>
   </si>
@@ -28,52 +28,13 @@
     <t>Time to insert (seconds)</t>
   </si>
   <si>
-    <t>Original file size</t>
-  </si>
-  <si>
-    <t>Size of database after insert</t>
-  </si>
-  <si>
     <t>Number of sequences</t>
   </si>
   <si>
-    <t>34.24 GB</t>
+    <t>Input FASTQ</t>
   </si>
   <si>
-    <t>68.12 GB</t>
-  </si>
-  <si>
-    <t>743 MB</t>
-  </si>
-  <si>
-    <t>1486 MB</t>
-  </si>
-  <si>
-    <t>2.98 GB</t>
-  </si>
-  <si>
-    <t>5.94 GB</t>
-  </si>
-  <si>
-    <t>11.88 GB</t>
-  </si>
-  <si>
-    <t>23.78 GB</t>
-  </si>
-  <si>
-    <t>47.56 GB</t>
-  </si>
-  <si>
-    <t>371.4 MB</t>
-  </si>
-  <si>
-    <t>258.6 MB</t>
-  </si>
-  <si>
-    <t>517.2 MB</t>
-  </si>
-  <si>
-    <t>1054.72 MB</t>
+    <t>Pip Database</t>
   </si>
 </sst>
 </file>
@@ -332,6 +293,279 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>sizes!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Input FASTQ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>sizes!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0E6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0E6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.0E6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>sizes!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>371.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>743.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1486.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3051.52</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6082.56</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12165.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>sizes!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pip Database</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>sizes!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0E6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0E6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.0E6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>sizes!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>206.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>413.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>828.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1699.84</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3389.44</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6789.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2106319992"/>
+        <c:axId val="-2106317720"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2106319992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of sequences</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2106317720"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2106317720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>File size (MB)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2106319992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -350,6 +584,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -785,113 +1054,123 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
         <v>500000</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
+      <c r="B2">
+        <v>371.4</v>
+      </c>
+      <c r="C2">
+        <v>206.9</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
         <v>1000000</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
+      <c r="B3">
+        <v>743</v>
+      </c>
+      <c r="C3">
+        <v>413.9</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
         <v>2000000</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
+      <c r="B4">
+        <v>1486</v>
+      </c>
+      <c r="C4">
+        <v>828</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
         <v>4000000</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
+      <c r="B5">
+        <v>3051.52</v>
+      </c>
+      <c r="C5">
+        <v>1699.84</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
         <v>8000000</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
+      <c r="B6">
+        <v>6082.56</v>
+      </c>
+      <c r="C6">
+        <v>3389.44</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
         <v>16000000</v>
       </c>
-      <c r="B7" t="s">
-        <v>11</v>
+      <c r="B7">
+        <v>12165.12</v>
+      </c>
+      <c r="C7">
+        <v>6789.12</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
         <v>32000000</v>
       </c>
-      <c r="B8" t="s">
-        <v>12</v>
+      <c r="B8">
+        <v>24350.720000000001</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
         <v>64000000</v>
       </c>
-      <c r="B9" t="s">
-        <v>13</v>
+      <c r="B9">
+        <v>48701.440000000002</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
         <v>91000000</v>
       </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
+      <c r="B10">
+        <v>69754.880000000005</v>
+      </c>
+      <c r="C10">
+        <v>35061.760000000002</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
renamed file size references, updated file size chart data.
</commit_message>
<xml_diff>
--- a/thesis/data and charts.xlsx
+++ b/thesis/data and charts.xlsx
@@ -331,10 +331,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>sizes!$A$2:$A$7</c:f>
+              <c:f>sizes!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>500000.0</c:v>
                 </c:pt>
@@ -352,16 +352,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.6E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.2E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>sizes!$B$2:$B$7</c:f>
+              <c:f>sizes!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>371.4</c:v>
                 </c:pt>
@@ -379,6 +382,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>12165.12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24350.72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -406,10 +412,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>sizes!$A$2:$A$7</c:f>
+              <c:f>sizes!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>500000.0</c:v>
                 </c:pt>
@@ -427,16 +433,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.6E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.2E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>sizes!$C$2:$C$7</c:f>
+              <c:f>sizes!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>206.9</c:v>
                 </c:pt>
@@ -454,6 +463,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6789.12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13568.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1054,7 +1066,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1148,6 +1160,9 @@
       <c r="B8">
         <v>24350.720000000001</v>
       </c>
+      <c r="C8">
+        <v>13568</v>
+      </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9">

</xml_diff>

<commit_message>
Completed results for file sizes.
</commit_message>
<xml_diff>
--- a/thesis/data and charts.xlsx
+++ b/thesis/data and charts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25580" windowHeight="28280" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25580" windowHeight="17480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="inserts" sheetId="1" r:id="rId1"/>
@@ -331,10 +331,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>sizes!$A$2:$A$8</c:f>
+              <c:f>sizes!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>500000.0</c:v>
                 </c:pt>
@@ -355,16 +355,22 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>3.2E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.4E7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.1E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>sizes!$B$2:$B$8</c:f>
+              <c:f>sizes!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>371.4</c:v>
                 </c:pt>
@@ -385,6 +391,12 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>24350.72</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>48701.44</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>69754.88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -412,10 +424,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>sizes!$A$2:$A$8</c:f>
+              <c:f>sizes!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>500000.0</c:v>
                 </c:pt>
@@ -436,16 +448,22 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>3.2E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.4E7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.1E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>sizes!$C$2:$C$8</c:f>
+              <c:f>sizes!$C$2:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>206.9</c:v>
                 </c:pt>
@@ -466,6 +484,12 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>13568.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27146.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35061.76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1065,8 +1089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1171,6 +1195,9 @@
       <c r="B9">
         <v>48701.440000000002</v>
       </c>
+      <c r="C9">
+        <v>27146.2</v>
+      </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">

</xml_diff>